<commit_message>
scripts to get logs
</commit_message>
<xml_diff>
--- a/benchmarks/results.xlsx
+++ b/benchmarks/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmb21/Papers/energise/benchmarks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84956137-7EA0-264A-9441-F002CB0BAF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC71669-DDCD-3F4A-9ACB-3324CBBC8FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13420" yWindow="760" windowWidth="15140" windowHeight="16700" xr2:uid="{427FDE2C-09F9-CD41-AE51-1D7613F79F67}"/>
+    <workbookView xWindow="11120" yWindow="760" windowWidth="19120" windowHeight="17300" xr2:uid="{427FDE2C-09F9-CD41-AE51-1D7613F79F67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>% Saving</t>
+  </si>
+  <si>
+    <t>book</t>
   </si>
 </sst>
 </file>
@@ -461,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F597843-20D4-424E-9B68-316E59443408}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -530,7 +533,7 @@
         <v>0.641984</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E13" si="0">C3*D3</f>
+        <f t="shared" ref="E3:E15" si="0">C3*D3</f>
         <v>77.142745861439991</v>
       </c>
       <c r="F3" s="1">
@@ -799,6 +802,51 @@
       <c r="I13">
         <f>100-(E13/E12*100)</f>
         <v>0.22479781840716839</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1">
+        <v>120.212642</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.16001899999999999</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>19.236306760198001</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3.7234020000000001</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.89367200000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1">
+        <v>120.96821</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.16462099999999999</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>19.91390769841</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.7715380000000001</v>
+      </c>
+      <c r="G15" s="1">
+        <v>47.312910000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>